<commit_message>
complete all statistics reported in the main text
</commit_message>
<xml_diff>
--- a/Longtan lithic data-Reaffutage.xlsx
+++ b/Longtan lithic data-Reaffutage.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Desktop\龙潭发掘Quina标本数据-2023.8\LT石制品数据\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Desktop\龙潭发掘Quina标本数据-2023.8\Lithic-data-Longtan-site\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BCA0439-D46A-4255-81FB-FDB913A23185}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C086BBA0-0C55-4E71-9443-00DAC4DD12B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" xr2:uid="{AFED09AC-7E11-4630-AF3B-9797082C5913}"/>
   </bookViews>
@@ -727,6 +727,24 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -739,28 +757,10 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1080,7 +1080,7 @@
   <dimension ref="A1:AZ61"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+      <selection activeCell="H2" sqref="H2:H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.640625" defaultRowHeight="18.45"/>
@@ -1100,60 +1100,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="28" t="s">
         <v>58</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="C1" s="28" t="s">
         <v>59</v>
       </c>
-      <c r="D1" s="24" t="s">
+      <c r="D1" s="28" t="s">
         <v>60</v>
       </c>
-      <c r="E1" s="24" t="s">
+      <c r="E1" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="F1" s="18" t="s">
+      <c r="F1" s="24" t="s">
         <v>62</v>
       </c>
-      <c r="G1" s="21" t="s">
+      <c r="G1" s="20" t="s">
         <v>63</v>
       </c>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
-      <c r="K1" s="21"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="20"/>
       <c r="L1" s="22" t="s">
         <v>70</v>
       </c>
       <c r="M1" s="22"/>
       <c r="N1" s="22"/>
-      <c r="O1" s="25" t="s">
+      <c r="O1" s="17" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:19">
-      <c r="A2" s="17"/>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="23" t="s">
+      <c r="A2" s="23"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="27" t="s">
         <v>64</v>
       </c>
-      <c r="H2" s="21" t="s">
+      <c r="H2" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="I2" s="21" t="s">
+      <c r="I2" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="J2" s="21" t="s">
+      <c r="J2" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="K2" s="28" t="s">
+      <c r="K2" s="21" t="s">
         <v>68</v>
       </c>
       <c r="L2" s="22" t="s">
@@ -1163,20 +1163,20 @@
       <c r="N2" s="22" t="s">
         <v>72</v>
       </c>
-      <c r="O2" s="26"/>
+      <c r="O2" s="18"/>
     </row>
     <row r="3" spans="1:19" ht="18" customHeight="1">
-      <c r="A3" s="17"/>
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="23"/>
-      <c r="H3" s="21"/>
-      <c r="I3" s="21"/>
-      <c r="J3" s="21"/>
-      <c r="K3" s="21"/>
+      <c r="A3" s="23"/>
+      <c r="B3" s="28"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="27"/>
+      <c r="H3" s="20"/>
+      <c r="I3" s="20"/>
+      <c r="J3" s="20"/>
+      <c r="K3" s="20"/>
       <c r="L3" s="22" t="s">
         <v>73</v>
       </c>
@@ -1184,24 +1184,24 @@
         <v>71</v>
       </c>
       <c r="N3" s="22"/>
-      <c r="O3" s="26"/>
+      <c r="O3" s="18"/>
     </row>
     <row r="4" spans="1:19" ht="18" customHeight="1">
-      <c r="A4" s="17"/>
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="23"/>
-      <c r="H4" s="21"/>
-      <c r="I4" s="21"/>
-      <c r="J4" s="21"/>
-      <c r="K4" s="21"/>
+      <c r="A4" s="23"/>
+      <c r="B4" s="28"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="28"/>
+      <c r="F4" s="26"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
+      <c r="K4" s="20"/>
       <c r="L4" s="22"/>
       <c r="M4" s="22"/>
       <c r="N4" s="22"/>
-      <c r="O4" s="27"/>
+      <c r="O4" s="19"/>
     </row>
     <row r="5" spans="1:19">
       <c r="A5" s="2" t="s">
@@ -4459,6 +4459,15 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A1:A4"/>
+    <mergeCell ref="F1:F4"/>
+    <mergeCell ref="G1:K1"/>
+    <mergeCell ref="L1:N1"/>
+    <mergeCell ref="G2:G4"/>
+    <mergeCell ref="E1:E4"/>
+    <mergeCell ref="D1:D4"/>
+    <mergeCell ref="C1:C4"/>
+    <mergeCell ref="B1:B4"/>
     <mergeCell ref="O1:O4"/>
     <mergeCell ref="H2:H4"/>
     <mergeCell ref="I2:I4"/>
@@ -4468,15 +4477,6 @@
     <mergeCell ref="N2:N4"/>
     <mergeCell ref="L3:L4"/>
     <mergeCell ref="M3:M4"/>
-    <mergeCell ref="A1:A4"/>
-    <mergeCell ref="F1:F4"/>
-    <mergeCell ref="G1:K1"/>
-    <mergeCell ref="L1:N1"/>
-    <mergeCell ref="G2:G4"/>
-    <mergeCell ref="E1:E4"/>
-    <mergeCell ref="D1:D4"/>
-    <mergeCell ref="C1:C4"/>
-    <mergeCell ref="B1:B4"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <dataValidations count="1">

</xml_diff>

<commit_message>
modify some details about plots
</commit_message>
<xml_diff>
--- a/Longtan lithic data-Reaffutage.xlsx
+++ b/Longtan lithic data-Reaffutage.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Desktop\龙潭发掘Quina标本数据-2023.8\Lithic-data-Longtan-site\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C086BBA0-0C55-4E71-9443-00DAC4DD12B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D979B0F8-79DA-465C-B0BD-284DBD74C13A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" xr2:uid="{AFED09AC-7E11-4630-AF3B-9797082C5913}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="90">
   <si>
     <t>19YHL-T2-3-L7:721</t>
   </si>
@@ -409,12 +409,20 @@
     </r>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
+  <si>
+    <t>DSP</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Proximal only</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -468,6 +476,14 @@
       <sz val="14"/>
       <color theme="1"/>
       <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="微软雅黑"/>
       <family val="3"/>
       <charset val="134"/>
     </font>
@@ -675,7 +691,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -727,24 +743,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -757,10 +755,37 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1077,10 +1102,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70BA2224-75CA-4FFA-93C6-6107C6F3A8FF}">
-  <dimension ref="A1:AZ61"/>
+  <dimension ref="A1:BA61"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H4"/>
+      <selection activeCell="O5" sqref="O5:O61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.640625" defaultRowHeight="18.45"/>
@@ -1094,66 +1119,69 @@
     <col min="7" max="11" width="8.640625" style="1"/>
     <col min="12" max="12" width="13.5703125" style="1" customWidth="1"/>
     <col min="13" max="13" width="8.640625" style="1"/>
-    <col min="14" max="14" width="18.5" style="1" customWidth="1"/>
-    <col min="15" max="15" width="9.2109375" style="1" customWidth="1"/>
-    <col min="16" max="16384" width="8.640625" style="1"/>
+    <col min="14" max="15" width="18.5" style="1" customWidth="1"/>
+    <col min="16" max="16" width="9.2109375" style="1" customWidth="1"/>
+    <col min="17" max="16384" width="8.640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19">
-      <c r="A1" s="23" t="s">
+    <row r="1" spans="1:20">
+      <c r="A1" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="C1" s="28" t="s">
+      <c r="C1" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="D1" s="28" t="s">
+      <c r="D1" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="E1" s="28" t="s">
+      <c r="E1" s="24" t="s">
         <v>61</v>
       </c>
-      <c r="F1" s="24" t="s">
+      <c r="F1" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="G1" s="20" t="s">
+      <c r="G1" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
       <c r="L1" s="22" t="s">
         <v>70</v>
       </c>
       <c r="M1" s="22"/>
       <c r="N1" s="22"/>
-      <c r="O1" s="17" t="s">
+      <c r="O1" s="31" t="s">
+        <v>88</v>
+      </c>
+      <c r="P1" s="25" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="2" spans="1:19">
-      <c r="A2" s="23"/>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="27" t="s">
+    <row r="2" spans="1:20">
+      <c r="A2" s="17"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="H2" s="20" t="s">
+      <c r="H2" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="I2" s="20" t="s">
+      <c r="I2" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="J2" s="20" t="s">
+      <c r="J2" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="K2" s="21" t="s">
+      <c r="K2" s="28" t="s">
         <v>68</v>
       </c>
       <c r="L2" s="22" t="s">
@@ -1163,20 +1191,21 @@
       <c r="N2" s="22" t="s">
         <v>72</v>
       </c>
-      <c r="O2" s="18"/>
-    </row>
-    <row r="3" spans="1:19" ht="18" customHeight="1">
-      <c r="A3" s="23"/>
-      <c r="B3" s="28"/>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="27"/>
-      <c r="H3" s="20"/>
-      <c r="I3" s="20"/>
-      <c r="J3" s="20"/>
-      <c r="K3" s="20"/>
+      <c r="O2" s="29"/>
+      <c r="P2" s="26"/>
+    </row>
+    <row r="3" spans="1:20" ht="18" customHeight="1">
+      <c r="A3" s="17"/>
+      <c r="B3" s="24"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="21"/>
+      <c r="J3" s="21"/>
+      <c r="K3" s="21"/>
       <c r="L3" s="22" t="s">
         <v>73</v>
       </c>
@@ -1184,26 +1213,28 @@
         <v>71</v>
       </c>
       <c r="N3" s="22"/>
-      <c r="O3" s="18"/>
-    </row>
-    <row r="4" spans="1:19" ht="18" customHeight="1">
-      <c r="A4" s="23"/>
-      <c r="B4" s="28"/>
-      <c r="C4" s="28"/>
-      <c r="D4" s="28"/>
-      <c r="E4" s="28"/>
-      <c r="F4" s="26"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="20"/>
-      <c r="J4" s="20"/>
-      <c r="K4" s="20"/>
+      <c r="O3" s="29"/>
+      <c r="P3" s="26"/>
+    </row>
+    <row r="4" spans="1:20" ht="18" customHeight="1">
+      <c r="A4" s="17"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="21"/>
+      <c r="I4" s="21"/>
+      <c r="J4" s="21"/>
+      <c r="K4" s="21"/>
       <c r="L4" s="22"/>
       <c r="M4" s="22"/>
       <c r="N4" s="22"/>
-      <c r="O4" s="19"/>
-    </row>
-    <row r="5" spans="1:19">
+      <c r="O4" s="30"/>
+      <c r="P4" s="27"/>
+    </row>
+    <row r="5" spans="1:20">
       <c r="A5" s="2" t="s">
         <v>0</v>
       </c>
@@ -1244,25 +1275,28 @@
       <c r="N5" s="7">
         <v>4</v>
       </c>
-      <c r="O5" s="2"/>
-      <c r="P5" s="1">
+      <c r="O5" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="P5" s="2"/>
+      <c r="Q5" s="1">
         <f>B5/C5</f>
         <v>1.1896435776731675</v>
       </c>
-      <c r="Q5" s="1">
+      <c r="R5" s="1">
         <f>H5*I5</f>
         <v>14.091000000000001</v>
       </c>
-      <c r="R5" s="1">
+      <c r="S5" s="1">
         <f>B5*C5*D5</f>
         <v>10816.628336</v>
       </c>
-      <c r="S5" s="1">
-        <f>Q5/R5</f>
+      <c r="T5" s="1">
+        <f>R5/S5</f>
         <v>1.3027164808004179E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:19">
+    <row r="6" spans="1:20">
       <c r="A6" s="3" t="s">
         <v>1</v>
       </c>
@@ -1303,25 +1337,28 @@
       <c r="N6" s="9">
         <v>3</v>
       </c>
-      <c r="O6" s="3"/>
-      <c r="P6" s="1">
-        <f t="shared" ref="P6:P61" si="0">B6/C6</f>
+      <c r="O6" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="1">
+        <f t="shared" ref="Q6:Q61" si="0">B6/C6</f>
         <v>1.2314874436574372</v>
       </c>
-      <c r="Q6" s="1">
-        <f t="shared" ref="Q6:Q60" si="1">H6*I6</f>
+      <c r="R6" s="1">
+        <f t="shared" ref="R6:R60" si="1">H6*I6</f>
         <v>31.774500000000003</v>
       </c>
-      <c r="R6" s="1">
-        <f t="shared" ref="R6:R61" si="2">B6*C6*D6</f>
+      <c r="S6" s="1">
+        <f t="shared" ref="S6:S61" si="2">B6*C6*D6</f>
         <v>8720.2502999999979</v>
       </c>
-      <c r="S6" s="1">
-        <f t="shared" ref="S6:S61" si="3">Q6/R6</f>
+      <c r="T6" s="1">
+        <f t="shared" ref="T6:T61" si="3">R6/S6</f>
         <v>3.6437600879415137E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:19">
+    <row r="7" spans="1:20">
       <c r="A7" s="3" t="s">
         <v>2</v>
       </c>
@@ -1351,13 +1388,16 @@
       <c r="N7" s="9">
         <v>4</v>
       </c>
-      <c r="O7" s="3"/>
-      <c r="P7" s="1">
+      <c r="O7" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="P7" s="3"/>
+      <c r="Q7" s="1">
         <f t="shared" si="0"/>
         <v>1.6346828179789608</v>
       </c>
     </row>
-    <row r="8" spans="1:19">
+    <row r="8" spans="1:20">
       <c r="A8" s="3" t="s">
         <v>3</v>
       </c>
@@ -1397,25 +1437,28 @@
       <c r="N8" s="9">
         <v>3</v>
       </c>
-      <c r="O8" s="3"/>
-      <c r="P8" s="1">
+      <c r="O8" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="P8" s="3"/>
+      <c r="Q8" s="1">
         <f t="shared" si="0"/>
         <v>1.2137096774193548</v>
       </c>
-      <c r="Q8" s="1">
+      <c r="R8" s="1">
         <f t="shared" si="1"/>
         <v>29.2864</v>
       </c>
-      <c r="R8" s="1">
+      <c r="S8" s="1">
         <f t="shared" si="2"/>
         <v>11254.529664</v>
       </c>
-      <c r="S8" s="1">
+      <c r="T8" s="1">
         <f t="shared" si="3"/>
         <v>2.602187818979123E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:19">
+    <row r="9" spans="1:20">
       <c r="A9" s="3" t="s">
         <v>5</v>
       </c>
@@ -1456,25 +1499,28 @@
       <c r="N9" s="9">
         <v>3</v>
       </c>
-      <c r="O9" s="3"/>
-      <c r="P9" s="1">
+      <c r="O9" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="P9" s="3"/>
+      <c r="Q9" s="1">
         <f t="shared" si="0"/>
         <v>0.99792339640055372</v>
       </c>
-      <c r="Q9" s="1">
+      <c r="R9" s="1">
         <f t="shared" si="1"/>
         <v>123.623</v>
       </c>
-      <c r="R9" s="1">
+      <c r="S9" s="1">
         <f t="shared" si="2"/>
         <v>26242.370000000003</v>
       </c>
-      <c r="S9" s="1">
+      <c r="T9" s="1">
         <f t="shared" si="3"/>
         <v>4.7108168964921995E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:19">
+    <row r="10" spans="1:20">
       <c r="A10" s="3" t="s">
         <v>6</v>
       </c>
@@ -1515,25 +1561,28 @@
       <c r="N10" s="9">
         <v>3</v>
       </c>
-      <c r="O10" s="3"/>
-      <c r="P10" s="1">
+      <c r="O10" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="P10" s="3"/>
+      <c r="Q10" s="1">
         <f t="shared" si="0"/>
         <v>1.1573236889692586</v>
       </c>
-      <c r="Q10" s="1">
+      <c r="R10" s="1">
         <f t="shared" si="1"/>
         <v>18.358599999999999</v>
       </c>
-      <c r="R10" s="1">
+      <c r="S10" s="1">
         <f t="shared" si="2"/>
         <v>4269.6908800000001</v>
       </c>
-      <c r="S10" s="1">
+      <c r="T10" s="1">
         <f t="shared" si="3"/>
         <v>4.2997492127579964E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:19">
+    <row r="11" spans="1:20">
       <c r="A11" s="3" t="s">
         <v>7</v>
       </c>
@@ -1573,25 +1622,28 @@
       <c r="N11" s="9">
         <v>3</v>
       </c>
-      <c r="O11" s="3"/>
-      <c r="P11" s="1">
+      <c r="O11" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="P11" s="3"/>
+      <c r="Q11" s="1">
         <f t="shared" si="0"/>
         <v>1.1563367252543941</v>
       </c>
-      <c r="Q11" s="1">
+      <c r="R11" s="1">
         <f t="shared" si="1"/>
         <v>22.113</v>
       </c>
-      <c r="R11" s="1">
+      <c r="S11" s="1">
         <f t="shared" si="2"/>
         <v>9558.7425000000003</v>
       </c>
-      <c r="S11" s="1">
+      <c r="T11" s="1">
         <f t="shared" si="3"/>
         <v>2.3133796103410043E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:19">
+    <row r="12" spans="1:20">
       <c r="A12" s="3" t="s">
         <v>9</v>
       </c>
@@ -1632,25 +1684,28 @@
       <c r="N12" s="9">
         <v>3</v>
       </c>
-      <c r="O12" s="3"/>
-      <c r="P12" s="1">
+      <c r="O12" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="P12" s="3"/>
+      <c r="Q12" s="1">
         <f t="shared" si="0"/>
         <v>1.2976234003656306</v>
       </c>
-      <c r="Q12" s="1">
+      <c r="R12" s="1">
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
-      <c r="R12" s="1">
+      <c r="S12" s="1">
         <f t="shared" si="2"/>
         <v>7726.3859400000001</v>
       </c>
-      <c r="S12" s="1">
+      <c r="T12" s="1">
         <f t="shared" si="3"/>
         <v>2.3296791203262102E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:19">
+    <row r="13" spans="1:20">
       <c r="A13" s="3" t="s">
         <v>10</v>
       </c>
@@ -1691,25 +1746,28 @@
       <c r="N13" s="9">
         <v>2</v>
       </c>
-      <c r="O13" s="3"/>
-      <c r="P13" s="1">
+      <c r="O13" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="P13" s="3"/>
+      <c r="Q13" s="1">
         <f t="shared" si="0"/>
         <v>1.3374549201442556</v>
       </c>
-      <c r="Q13" s="1">
+      <c r="R13" s="1">
         <f t="shared" si="1"/>
         <v>27.454800000000002</v>
       </c>
-      <c r="R13" s="1">
+      <c r="S13" s="1">
         <f t="shared" si="2"/>
         <v>3083.767632</v>
       </c>
-      <c r="S13" s="1">
+      <c r="T13" s="1">
         <f t="shared" si="3"/>
         <v>8.9030054389000746E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:19">
+    <row r="14" spans="1:20">
       <c r="A14" s="3" t="s">
         <v>11</v>
       </c>
@@ -1750,25 +1808,28 @@
       <c r="N14" s="9">
         <v>3</v>
       </c>
-      <c r="O14" s="3"/>
-      <c r="P14" s="1">
+      <c r="O14" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="P14" s="3"/>
+      <c r="Q14" s="1">
         <f t="shared" si="0"/>
         <v>1.3684868695289705</v>
       </c>
-      <c r="Q14" s="1">
+      <c r="R14" s="1">
         <f t="shared" si="1"/>
         <v>33.490799999999993</v>
       </c>
-      <c r="R14" s="1">
+      <c r="S14" s="1">
         <f t="shared" si="2"/>
         <v>7332.4787269999997</v>
       </c>
-      <c r="S14" s="1">
+      <c r="T14" s="1">
         <f t="shared" si="3"/>
         <v>4.5674595517991188E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:19">
+    <row r="15" spans="1:20">
       <c r="A15" s="3" t="s">
         <v>12</v>
       </c>
@@ -1808,25 +1869,28 @@
       <c r="N15" s="9">
         <v>3</v>
       </c>
-      <c r="O15" s="3"/>
-      <c r="P15" s="1">
+      <c r="O15" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="P15" s="3"/>
+      <c r="Q15" s="1">
         <f t="shared" si="0"/>
         <v>1.1785037878787878</v>
       </c>
-      <c r="Q15" s="1">
+      <c r="R15" s="1">
         <f t="shared" si="1"/>
         <v>8.4600000000000009</v>
       </c>
-      <c r="R15" s="1">
+      <c r="S15" s="1">
         <f t="shared" si="2"/>
         <v>3222.3987840000004</v>
       </c>
-      <c r="S15" s="1">
+      <c r="T15" s="1">
         <f t="shared" si="3"/>
         <v>2.6253733839542064E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:19">
+    <row r="16" spans="1:20">
       <c r="A16" s="3" t="s">
         <v>13</v>
       </c>
@@ -1867,25 +1931,28 @@
       <c r="N16" s="9">
         <v>3</v>
       </c>
-      <c r="O16" s="3"/>
-      <c r="P16" s="1">
+      <c r="O16" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="P16" s="3"/>
+      <c r="Q16" s="1">
         <f t="shared" si="0"/>
         <v>1.1357142857142857</v>
       </c>
-      <c r="Q16" s="1">
+      <c r="R16" s="1">
         <f t="shared" si="1"/>
         <v>4.2349999999999994</v>
       </c>
-      <c r="R16" s="1">
+      <c r="S16" s="1">
         <f t="shared" si="2"/>
         <v>2547.9686400000001</v>
       </c>
-      <c r="S16" s="1">
+      <c r="T16" s="1">
         <f t="shared" si="3"/>
         <v>1.6621083688062972E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:19">
+    <row r="17" spans="1:20">
       <c r="A17" s="3" t="s">
         <v>14</v>
       </c>
@@ -1926,25 +1993,28 @@
       <c r="N17" s="9">
         <v>1</v>
       </c>
-      <c r="O17" s="3"/>
-      <c r="P17" s="1">
+      <c r="O17" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="P17" s="3"/>
+      <c r="Q17" s="1">
         <f t="shared" si="0"/>
         <v>1.0481099656357387</v>
       </c>
-      <c r="Q17" s="1">
+      <c r="R17" s="1">
         <f t="shared" si="1"/>
         <v>43.2896</v>
       </c>
-      <c r="R17" s="1">
+      <c r="S17" s="1">
         <f t="shared" si="2"/>
         <v>2982.1680000000001</v>
       </c>
-      <c r="S17" s="1">
+      <c r="T17" s="1">
         <f t="shared" si="3"/>
         <v>1.4516150666226718E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:19">
+    <row r="18" spans="1:20">
       <c r="A18" s="3" t="s">
         <v>15</v>
       </c>
@@ -1985,25 +2055,28 @@
       <c r="N18" s="9">
         <v>3</v>
       </c>
-      <c r="O18" s="3"/>
-      <c r="P18" s="1">
+      <c r="O18" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="P18" s="3"/>
+      <c r="Q18" s="1">
         <f t="shared" si="0"/>
         <v>1.2391942929080992</v>
       </c>
-      <c r="Q18" s="1">
+      <c r="R18" s="1">
         <f t="shared" si="1"/>
         <v>16.912700000000001</v>
       </c>
-      <c r="R18" s="1">
+      <c r="S18" s="1">
         <f t="shared" si="2"/>
         <v>4306.6433879999995</v>
       </c>
-      <c r="S18" s="1">
+      <c r="T18" s="1">
         <f t="shared" si="3"/>
         <v>3.9271187503301126E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:19">
+    <row r="19" spans="1:20">
       <c r="A19" s="3" t="s">
         <v>16</v>
       </c>
@@ -2044,25 +2117,28 @@
       <c r="N19" s="9">
         <v>3</v>
       </c>
-      <c r="O19" s="3"/>
-      <c r="P19" s="1">
+      <c r="O19" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="P19" s="3"/>
+      <c r="Q19" s="1">
         <f t="shared" si="0"/>
         <v>1.3080739738385205</v>
       </c>
-      <c r="Q19" s="1">
+      <c r="R19" s="1">
         <f t="shared" si="1"/>
         <v>39.428400000000003</v>
       </c>
-      <c r="R19" s="1">
+      <c r="S19" s="1">
         <f t="shared" si="2"/>
         <v>4680.5304000000006</v>
       </c>
-      <c r="S19" s="1">
+      <c r="T19" s="1">
         <f t="shared" si="3"/>
         <v>8.4239170842689108E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:19">
+    <row r="20" spans="1:20">
       <c r="A20" s="3" t="s">
         <v>17</v>
       </c>
@@ -2102,25 +2178,28 @@
       <c r="N20" s="9">
         <v>2</v>
       </c>
-      <c r="O20" s="3"/>
-      <c r="P20" s="1">
+      <c r="O20" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="P20" s="3"/>
+      <c r="Q20" s="1">
         <f t="shared" si="0"/>
         <v>1.0497328401150843</v>
       </c>
-      <c r="Q20" s="1">
+      <c r="R20" s="1">
         <f t="shared" si="1"/>
         <v>36.481999999999999</v>
       </c>
-      <c r="R20" s="1">
+      <c r="S20" s="1">
         <f t="shared" si="2"/>
         <v>3231.2186400000001</v>
       </c>
-      <c r="S20" s="1">
+      <c r="T20" s="1">
         <f t="shared" si="3"/>
         <v>1.1290477081427086E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:19">
+    <row r="21" spans="1:20">
       <c r="A21" s="3" t="s">
         <v>18</v>
       </c>
@@ -2161,25 +2240,28 @@
       <c r="N21" s="9">
         <v>2</v>
       </c>
-      <c r="O21" s="3"/>
-      <c r="P21" s="1">
+      <c r="O21" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="P21" s="3"/>
+      <c r="Q21" s="1">
         <f t="shared" si="0"/>
         <v>1.0931707317073172</v>
       </c>
-      <c r="Q21" s="1">
+      <c r="R21" s="1">
         <f t="shared" si="1"/>
         <v>67.7286</v>
       </c>
-      <c r="R21" s="1">
+      <c r="S21" s="1">
         <f t="shared" si="2"/>
         <v>2811.5586000000003</v>
       </c>
-      <c r="S21" s="1">
+      <c r="T21" s="1">
         <f t="shared" si="3"/>
         <v>2.4089343184950863E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:19">
+    <row r="22" spans="1:20">
       <c r="A22" s="3" t="s">
         <v>19</v>
       </c>
@@ -2220,25 +2302,28 @@
       <c r="N22" s="9">
         <v>3</v>
       </c>
-      <c r="O22" s="3"/>
-      <c r="P22" s="1">
+      <c r="O22" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="P22" s="3"/>
+      <c r="Q22" s="1">
         <f t="shared" si="0"/>
         <v>1.1402439024390245</v>
       </c>
-      <c r="Q22" s="1">
+      <c r="R22" s="1">
         <f t="shared" si="1"/>
         <v>29.892999999999997</v>
       </c>
-      <c r="R22" s="1">
+      <c r="S22" s="1">
         <f t="shared" si="2"/>
         <v>2927.9352960000001</v>
       </c>
-      <c r="S22" s="1">
+      <c r="T22" s="1">
         <f t="shared" si="3"/>
         <v>1.0209583538556445E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:19">
+    <row r="23" spans="1:20">
       <c r="A23" s="3" t="s">
         <v>20</v>
       </c>
@@ -2279,25 +2364,28 @@
       <c r="N23" s="9">
         <v>3</v>
       </c>
-      <c r="O23" s="3"/>
-      <c r="P23" s="1">
+      <c r="O23" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="P23" s="3"/>
+      <c r="Q23" s="1">
         <f t="shared" si="0"/>
         <v>1.120860927152318</v>
       </c>
-      <c r="Q23" s="1">
+      <c r="R23" s="1">
         <f t="shared" si="1"/>
         <v>37.461600000000004</v>
       </c>
-      <c r="R23" s="1">
+      <c r="S23" s="1">
         <f t="shared" si="2"/>
         <v>8443.9501999999993</v>
       </c>
-      <c r="S23" s="1">
+      <c r="T23" s="1">
         <f t="shared" si="3"/>
         <v>4.4365017690416991E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:19">
+    <row r="24" spans="1:20">
       <c r="A24" s="3" t="s">
         <v>21</v>
       </c>
@@ -2338,25 +2426,28 @@
       <c r="N24" s="9">
         <v>2</v>
       </c>
-      <c r="O24" s="3"/>
-      <c r="P24" s="1">
+      <c r="O24" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="P24" s="3"/>
+      <c r="Q24" s="1">
         <f t="shared" si="0"/>
         <v>1.3647058823529412</v>
       </c>
-      <c r="Q24" s="1">
+      <c r="R24" s="1">
         <f t="shared" si="1"/>
         <v>59.445599999999992</v>
       </c>
-      <c r="R24" s="1">
+      <c r="S24" s="1">
         <f t="shared" si="2"/>
         <v>5262.7749999999996</v>
       </c>
-      <c r="S24" s="1">
+      <c r="T24" s="1">
         <f t="shared" si="3"/>
         <v>1.1295485746588063E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:19">
+    <row r="25" spans="1:20">
       <c r="A25" s="3" t="s">
         <v>22</v>
       </c>
@@ -2397,25 +2488,28 @@
       <c r="N25" s="9">
         <v>4</v>
       </c>
-      <c r="O25" s="3"/>
-      <c r="P25" s="1">
+      <c r="O25" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="P25" s="3"/>
+      <c r="Q25" s="1">
         <f t="shared" si="0"/>
         <v>1.9210754553339116</v>
       </c>
-      <c r="Q25" s="1">
+      <c r="R25" s="1">
         <f t="shared" si="1"/>
         <v>21.271799999999999</v>
       </c>
-      <c r="R25" s="1">
+      <c r="S25" s="1">
         <f t="shared" si="2"/>
         <v>11237.137999999999</v>
       </c>
-      <c r="S25" s="1">
+      <c r="T25" s="1">
         <f t="shared" si="3"/>
         <v>1.8929909021318419E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:19">
+    <row r="26" spans="1:20">
       <c r="A26" s="3" t="s">
         <v>23</v>
       </c>
@@ -2456,25 +2550,28 @@
       <c r="N26" s="9">
         <v>3</v>
       </c>
-      <c r="O26" s="3"/>
-      <c r="P26" s="1">
+      <c r="O26" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="P26" s="3"/>
+      <c r="Q26" s="1">
         <f t="shared" si="0"/>
         <v>1.7213225371120109</v>
       </c>
-      <c r="Q26" s="1">
+      <c r="R26" s="1">
         <f t="shared" si="1"/>
         <v>15.9</v>
       </c>
-      <c r="R26" s="1">
+      <c r="S26" s="1">
         <f t="shared" si="2"/>
         <v>1739.0677200000002</v>
       </c>
-      <c r="S26" s="1">
+      <c r="T26" s="1">
         <f t="shared" si="3"/>
         <v>9.1428296995817952E-3</v>
       </c>
     </row>
-    <row r="27" spans="1:19">
+    <row r="27" spans="1:20">
       <c r="A27" s="3" t="s">
         <v>24</v>
       </c>
@@ -2514,25 +2611,28 @@
       <c r="N27" s="9">
         <v>3</v>
       </c>
-      <c r="O27" s="3"/>
-      <c r="P27" s="1">
+      <c r="O27" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="P27" s="3"/>
+      <c r="Q27" s="1">
         <f t="shared" si="0"/>
         <v>1.0193838698511595</v>
       </c>
-      <c r="Q27" s="1">
+      <c r="R27" s="1">
         <f t="shared" si="1"/>
         <v>6.4295</v>
       </c>
-      <c r="R27" s="1">
+      <c r="S27" s="1">
         <f t="shared" si="2"/>
         <v>6636.3218999999999</v>
       </c>
-      <c r="S27" s="1">
+      <c r="T27" s="1">
         <f t="shared" si="3"/>
         <v>9.6883486016553842E-4</v>
       </c>
     </row>
-    <row r="28" spans="1:19">
+    <row r="28" spans="1:20">
       <c r="A28" s="3" t="s">
         <v>25</v>
       </c>
@@ -2573,25 +2673,28 @@
       <c r="N28" s="9">
         <v>3</v>
       </c>
-      <c r="O28" s="3"/>
-      <c r="P28" s="1">
+      <c r="O28" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="P28" s="3"/>
+      <c r="Q28" s="1">
         <f t="shared" si="0"/>
         <v>2.4353859496964438</v>
       </c>
-      <c r="Q28" s="1">
+      <c r="R28" s="1">
         <f t="shared" si="1"/>
         <v>71.104799999999997</v>
       </c>
-      <c r="R28" s="1">
+      <c r="S28" s="1">
         <f t="shared" si="2"/>
         <v>2444.4061199999996</v>
       </c>
-      <c r="S28" s="1">
+      <c r="T28" s="1">
         <f t="shared" si="3"/>
         <v>2.9088783331961222E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:19">
+    <row r="29" spans="1:20">
       <c r="A29" s="3" t="s">
         <v>26</v>
       </c>
@@ -2632,25 +2735,28 @@
       <c r="N29" s="9">
         <v>3</v>
       </c>
-      <c r="O29" s="3"/>
-      <c r="P29" s="1">
+      <c r="O29" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="P29" s="3"/>
+      <c r="Q29" s="1">
         <f t="shared" si="0"/>
         <v>1.5493942218080148</v>
       </c>
-      <c r="Q29" s="1">
+      <c r="R29" s="1">
         <f t="shared" si="1"/>
         <v>129.5625</v>
       </c>
-      <c r="R29" s="1">
+      <c r="S29" s="1">
         <f t="shared" si="2"/>
         <v>8113.0066500000003</v>
       </c>
-      <c r="S29" s="1">
+      <c r="T29" s="1">
         <f t="shared" si="3"/>
         <v>1.5969726833639411E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:19">
+    <row r="30" spans="1:20">
       <c r="A30" s="3" t="s">
         <v>27</v>
       </c>
@@ -2691,25 +2797,28 @@
       <c r="N30" s="9">
         <v>3</v>
       </c>
-      <c r="O30" s="3"/>
-      <c r="P30" s="1">
+      <c r="O30" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="P30" s="3"/>
+      <c r="Q30" s="1">
         <f t="shared" si="0"/>
         <v>1.2579225352112675</v>
       </c>
-      <c r="Q30" s="1">
+      <c r="R30" s="1">
         <f t="shared" si="1"/>
         <v>5.8097000000000003</v>
       </c>
-      <c r="R30" s="1">
+      <c r="S30" s="1">
         <f t="shared" si="2"/>
         <v>4636.2704639999993</v>
       </c>
-      <c r="S30" s="1">
+      <c r="T30" s="1">
         <f t="shared" si="3"/>
         <v>1.2530977312716156E-3</v>
       </c>
     </row>
-    <row r="31" spans="1:19">
+    <row r="31" spans="1:20">
       <c r="A31" s="3" t="s">
         <v>28</v>
       </c>
@@ -2750,25 +2859,28 @@
       <c r="N31" s="9">
         <v>2</v>
       </c>
-      <c r="O31" s="3"/>
-      <c r="P31" s="1">
+      <c r="O31" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="P31" s="3"/>
+      <c r="Q31" s="1">
         <f t="shared" si="0"/>
         <v>1.1102907245039224</v>
       </c>
-      <c r="Q31" s="1">
+      <c r="R31" s="1">
         <f t="shared" si="1"/>
         <v>53.456299999999999</v>
       </c>
-      <c r="R31" s="1">
+      <c r="S31" s="1">
         <f t="shared" si="2"/>
         <v>3675.7304100000001</v>
       </c>
-      <c r="S31" s="1">
+      <c r="T31" s="1">
         <f t="shared" si="3"/>
         <v>1.4543041528445499E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:19">
+    <row r="32" spans="1:20">
       <c r="A32" s="3" t="s">
         <v>29</v>
       </c>
@@ -2809,25 +2921,28 @@
       <c r="N32" s="9">
         <v>3</v>
       </c>
-      <c r="O32" s="3"/>
-      <c r="P32" s="1">
+      <c r="O32" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="P32" s="3"/>
+      <c r="Q32" s="1">
         <f t="shared" si="0"/>
         <v>1.5837424986361159</v>
       </c>
-      <c r="Q32" s="1">
+      <c r="R32" s="1">
         <f t="shared" si="1"/>
         <v>28.346399999999999</v>
       </c>
-      <c r="R32" s="1">
+      <c r="S32" s="1">
         <f t="shared" si="2"/>
         <v>3607.7729219999997</v>
       </c>
-      <c r="S32" s="1">
+      <c r="T32" s="1">
         <f t="shared" si="3"/>
         <v>7.8570355210399248E-3</v>
       </c>
     </row>
-    <row r="33" spans="1:52">
+    <row r="33" spans="1:53">
       <c r="A33" s="3" t="s">
         <v>30</v>
       </c>
@@ -2868,25 +2983,28 @@
       <c r="N33" s="9">
         <v>2</v>
       </c>
-      <c r="O33" s="3"/>
-      <c r="P33" s="1">
+      <c r="O33" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="P33" s="3"/>
+      <c r="Q33" s="1">
         <f t="shared" si="0"/>
         <v>1.4823923979877025</v>
       </c>
-      <c r="Q33" s="1">
+      <c r="R33" s="1">
         <f t="shared" si="1"/>
         <v>118.85130000000001</v>
       </c>
-      <c r="R33" s="1">
+      <c r="S33" s="1">
         <f t="shared" si="2"/>
         <v>3368.5438800000002</v>
       </c>
-      <c r="S33" s="1">
+      <c r="T33" s="1">
         <f t="shared" si="3"/>
         <v>3.528269312614684E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:52" ht="21">
+    <row r="34" spans="1:53" ht="21">
       <c r="A34" s="3" t="s">
         <v>84</v>
       </c>
@@ -2927,27 +3045,30 @@
       <c r="N34" s="9">
         <v>2</v>
       </c>
-      <c r="O34" s="3" t="s">
+      <c r="O34" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="P34" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="P34" s="1">
+      <c r="Q34" s="1">
         <f t="shared" si="0"/>
         <v>1.2820069204152249</v>
       </c>
-      <c r="Q34" s="1">
+      <c r="R34" s="1">
         <f t="shared" si="1"/>
         <v>100.548</v>
       </c>
-      <c r="R34" s="1">
+      <c r="S34" s="1">
         <f t="shared" si="2"/>
         <v>2852.4646800000005</v>
       </c>
-      <c r="S34" s="1">
+      <c r="T34" s="1">
         <f t="shared" si="3"/>
         <v>3.5249516218374341E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:52" ht="21">
+    <row r="35" spans="1:53" ht="21">
       <c r="A35" s="3" t="s">
         <v>85</v>
       </c>
@@ -2987,25 +3108,28 @@
       <c r="N35" s="9">
         <v>2</v>
       </c>
-      <c r="O35" s="3"/>
-      <c r="P35" s="1">
+      <c r="O35" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="P35" s="3"/>
+      <c r="Q35" s="1">
         <f t="shared" si="0"/>
         <v>2.0812704343764596</v>
       </c>
-      <c r="Q35" s="1">
+      <c r="R35" s="1">
         <f t="shared" si="1"/>
         <v>588.23440000000005</v>
       </c>
-      <c r="R35" s="1">
+      <c r="S35" s="1">
         <f t="shared" si="2"/>
         <v>14692.055840000001</v>
       </c>
-      <c r="S35" s="1">
+      <c r="T35" s="1">
         <f t="shared" si="3"/>
         <v>4.0037582650516254E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:52" ht="21">
+    <row r="36" spans="1:53" ht="21">
       <c r="A36" s="3" t="s">
         <v>86</v>
       </c>
@@ -3046,40 +3170,43 @@
       <c r="N36" s="9">
         <v>2</v>
       </c>
-      <c r="O36" s="3"/>
-      <c r="P36" s="1">
+      <c r="O36" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="P36" s="3"/>
+      <c r="Q36" s="1">
         <f t="shared" si="0"/>
         <v>1.5784681306909478</v>
       </c>
-      <c r="Q36" s="1">
+      <c r="R36" s="1">
         <f t="shared" si="1"/>
         <v>167.88200000000001</v>
       </c>
-      <c r="R36" s="1">
+      <c r="S36" s="1">
         <f t="shared" si="2"/>
         <v>4478.6678860000011</v>
       </c>
-      <c r="S36" s="1">
+      <c r="T36" s="1">
         <f t="shared" si="3"/>
         <v>3.7484806704419248E-2</v>
       </c>
-      <c r="AT36" s="1" t="s">
+      <c r="AU36" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AU36" s="1" t="s">
+      <c r="AV36" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="AV36" s="1">
-        <v>0</v>
       </c>
       <c r="AW36" s="1">
         <v>0</v>
       </c>
-      <c r="AZ36" s="1" t="e">
+      <c r="AX36" s="1">
+        <v>0</v>
+      </c>
+      <c r="BA36" s="1" t="e">
         <v>#REF!</v>
       </c>
     </row>
-    <row r="37" spans="1:52" ht="21">
+    <row r="37" spans="1:53" ht="21">
       <c r="A37" s="3" t="s">
         <v>87</v>
       </c>
@@ -3119,25 +3246,28 @@
       <c r="N37" s="9">
         <v>1</v>
       </c>
-      <c r="O37" s="3"/>
-      <c r="P37" s="1">
+      <c r="O37" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="P37" s="3"/>
+      <c r="Q37" s="1">
         <f t="shared" si="0"/>
         <v>1.5368324125230204</v>
       </c>
-      <c r="Q37" s="1">
+      <c r="R37" s="1">
         <f t="shared" si="1"/>
         <v>36.064000000000007</v>
       </c>
-      <c r="R37" s="1">
+      <c r="S37" s="1">
         <f t="shared" si="2"/>
         <v>5249.0984639999997</v>
       </c>
-      <c r="S37" s="1">
+      <c r="T37" s="1">
         <f t="shared" si="3"/>
         <v>6.8705131457027302E-3</v>
       </c>
     </row>
-    <row r="38" spans="1:52">
+    <row r="38" spans="1:53">
       <c r="A38" s="3" t="s">
         <v>33</v>
       </c>
@@ -3178,25 +3308,28 @@
       <c r="N38" s="9">
         <v>2</v>
       </c>
-      <c r="O38" s="3"/>
-      <c r="P38" s="1">
+      <c r="O38" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="P38" s="3"/>
+      <c r="Q38" s="1">
         <f t="shared" si="0"/>
         <v>1.4582023884349464</v>
       </c>
-      <c r="Q38" s="1">
+      <c r="R38" s="1">
         <f t="shared" si="1"/>
         <v>98.133099999999985</v>
       </c>
-      <c r="R38" s="1">
+      <c r="S38" s="1">
         <f t="shared" si="2"/>
         <v>2295.8766399999995</v>
       </c>
-      <c r="S38" s="1">
+      <c r="T38" s="1">
         <f t="shared" si="3"/>
         <v>4.2743193728387779E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:52">
+    <row r="39" spans="1:53">
       <c r="A39" s="3" t="s">
         <v>34</v>
       </c>
@@ -3237,25 +3370,28 @@
       <c r="N39" s="9">
         <v>3</v>
       </c>
-      <c r="O39" s="3"/>
-      <c r="P39" s="1">
+      <c r="O39" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="P39" s="3"/>
+      <c r="Q39" s="1">
         <f t="shared" si="0"/>
         <v>1.6175790285273708</v>
       </c>
-      <c r="Q39" s="1">
+      <c r="R39" s="1">
         <f t="shared" si="1"/>
         <v>237.39479999999998</v>
       </c>
-      <c r="R39" s="1">
+      <c r="S39" s="1">
         <f t="shared" si="2"/>
         <v>16010.987704000003</v>
       </c>
-      <c r="S39" s="1">
+      <c r="T39" s="1">
         <f t="shared" si="3"/>
         <v>1.4826992836968575E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:52">
+    <row r="40" spans="1:53">
       <c r="A40" s="3" t="s">
         <v>35</v>
       </c>
@@ -3296,25 +3432,28 @@
       <c r="N40" s="9">
         <v>2</v>
       </c>
-      <c r="O40" s="3"/>
-      <c r="P40" s="1">
+      <c r="O40" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="P40" s="3"/>
+      <c r="Q40" s="1">
         <f t="shared" si="0"/>
         <v>1.3077469793887704</v>
       </c>
-      <c r="Q40" s="1">
+      <c r="R40" s="1">
         <f t="shared" si="1"/>
         <v>7.3944000000000001</v>
       </c>
-      <c r="R40" s="1">
+      <c r="S40" s="1">
         <f t="shared" si="2"/>
         <v>1105.4517599999997</v>
       </c>
-      <c r="S40" s="1">
+      <c r="T40" s="1">
         <f t="shared" si="3"/>
         <v>6.6890300124900996E-3</v>
       </c>
     </row>
-    <row r="41" spans="1:52">
+    <row r="41" spans="1:53">
       <c r="A41" s="3" t="s">
         <v>36</v>
       </c>
@@ -3355,25 +3494,28 @@
       <c r="N41" s="9">
         <v>1</v>
       </c>
-      <c r="O41" s="3"/>
-      <c r="P41" s="1">
+      <c r="O41" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="P41" s="3"/>
+      <c r="Q41" s="1">
         <f t="shared" si="0"/>
         <v>1.4669365721997301</v>
       </c>
-      <c r="Q41" s="1">
+      <c r="R41" s="1">
         <f t="shared" si="1"/>
         <v>152.3792</v>
       </c>
-      <c r="R41" s="1">
+      <c r="S41" s="1">
         <f t="shared" si="2"/>
         <v>2090.9923320000003</v>
       </c>
-      <c r="S41" s="1">
+      <c r="T41" s="1">
         <f t="shared" si="3"/>
         <v>7.2874107507726618E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:52">
+    <row r="42" spans="1:53">
       <c r="A42" s="3" t="s">
         <v>37</v>
       </c>
@@ -3413,25 +3555,28 @@
       <c r="N42" s="9">
         <v>2</v>
       </c>
-      <c r="O42" s="3"/>
-      <c r="P42" s="1">
+      <c r="O42" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="P42" s="3"/>
+      <c r="Q42" s="1">
         <f t="shared" si="0"/>
         <v>1.592711682743837</v>
       </c>
-      <c r="Q42" s="1">
+      <c r="R42" s="1">
         <f t="shared" si="1"/>
         <v>265.53740000000005</v>
       </c>
-      <c r="R42" s="1">
+      <c r="S42" s="1">
         <f t="shared" si="2"/>
         <v>4713.8891999999996</v>
       </c>
-      <c r="S42" s="1">
+      <c r="T42" s="1">
         <f t="shared" si="3"/>
         <v>5.6330853088358564E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:52">
+    <row r="43" spans="1:53">
       <c r="A43" s="3" t="s">
         <v>38</v>
       </c>
@@ -3472,25 +3617,28 @@
       <c r="N43" s="9">
         <v>2</v>
       </c>
-      <c r="O43" s="3"/>
-      <c r="P43" s="1">
+      <c r="O43" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="P43" s="3"/>
+      <c r="Q43" s="1">
         <f t="shared" si="0"/>
         <v>1.2200630252100841</v>
       </c>
-      <c r="Q43" s="1">
+      <c r="R43" s="1">
         <f t="shared" si="1"/>
         <v>73.748999999999995</v>
       </c>
-      <c r="R43" s="1">
+      <c r="S43" s="1">
         <f t="shared" si="2"/>
         <v>3038.5955039999999</v>
       </c>
-      <c r="S43" s="1">
+      <c r="T43" s="1">
         <f t="shared" si="3"/>
         <v>2.427075268916741E-2</v>
       </c>
     </row>
-    <row r="44" spans="1:52">
+    <row r="44" spans="1:53">
       <c r="A44" s="3" t="s">
         <v>39</v>
       </c>
@@ -3531,25 +3679,28 @@
       <c r="N44" s="9">
         <v>3</v>
       </c>
-      <c r="O44" s="3"/>
-      <c r="P44" s="1">
+      <c r="O44" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="P44" s="3"/>
+      <c r="Q44" s="1">
         <f t="shared" si="0"/>
         <v>1.15809604759881</v>
       </c>
-      <c r="Q44" s="1">
+      <c r="R44" s="1">
         <f t="shared" si="1"/>
         <v>15.584800000000001</v>
       </c>
-      <c r="R44" s="1">
+      <c r="S44" s="1">
         <f t="shared" si="2"/>
         <v>3795.8595999999998</v>
       </c>
-      <c r="S44" s="1">
+      <c r="T44" s="1">
         <f t="shared" si="3"/>
         <v>4.1057366821470433E-3</v>
       </c>
     </row>
-    <row r="45" spans="1:52">
+    <row r="45" spans="1:53">
       <c r="A45" s="3" t="s">
         <v>40</v>
       </c>
@@ -3590,25 +3741,28 @@
       <c r="N45" s="9">
         <v>2</v>
       </c>
-      <c r="O45" s="3"/>
-      <c r="P45" s="1">
+      <c r="O45" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="P45" s="3"/>
+      <c r="Q45" s="1">
         <f t="shared" si="0"/>
         <v>1.0676345609065157</v>
       </c>
-      <c r="Q45" s="1">
+      <c r="R45" s="1">
         <f t="shared" si="1"/>
         <v>81.210899999999995</v>
       </c>
-      <c r="R45" s="1">
+      <c r="S45" s="1">
         <f t="shared" si="2"/>
         <v>10234.260719999998</v>
       </c>
-      <c r="S45" s="1">
+      <c r="T45" s="1">
         <f t="shared" si="3"/>
         <v>7.9351994464334896E-3</v>
       </c>
     </row>
-    <row r="46" spans="1:52">
+    <row r="46" spans="1:53">
       <c r="A46" s="3" t="s">
         <v>41</v>
       </c>
@@ -3648,25 +3802,28 @@
       <c r="N46" s="9">
         <v>2</v>
       </c>
-      <c r="O46" s="3"/>
-      <c r="P46" s="1">
+      <c r="O46" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="P46" s="3"/>
+      <c r="Q46" s="1">
         <f t="shared" si="0"/>
         <v>1.2520930232558141</v>
       </c>
-      <c r="Q46" s="1">
+      <c r="R46" s="1">
         <f t="shared" si="1"/>
         <v>361.64639999999997</v>
       </c>
-      <c r="R46" s="1">
+      <c r="S46" s="1">
         <f t="shared" si="2"/>
         <v>7784.5910000000003</v>
       </c>
-      <c r="S46" s="1">
+      <c r="T46" s="1">
         <f t="shared" si="3"/>
         <v>4.6456698881161509E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:52">
+    <row r="47" spans="1:53">
       <c r="A47" s="3" t="s">
         <v>42</v>
       </c>
@@ -3707,25 +3864,28 @@
       <c r="N47" s="9">
         <v>3</v>
       </c>
-      <c r="O47" s="3"/>
-      <c r="P47" s="1">
+      <c r="O47" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="P47" s="3"/>
+      <c r="Q47" s="1">
         <f t="shared" si="0"/>
         <v>1.7925336597307222</v>
       </c>
-      <c r="Q47" s="1">
+      <c r="R47" s="1">
         <f t="shared" si="1"/>
         <v>25.607400000000002</v>
       </c>
-      <c r="R47" s="1">
+      <c r="S47" s="1">
         <f t="shared" si="2"/>
         <v>4608.9045180000003</v>
       </c>
-      <c r="S47" s="1">
+      <c r="T47" s="1">
         <f t="shared" si="3"/>
         <v>5.5560708406934287E-3</v>
       </c>
     </row>
-    <row r="48" spans="1:52">
+    <row r="48" spans="1:53">
       <c r="A48" s="3" t="s">
         <v>43</v>
       </c>
@@ -3754,13 +3914,16 @@
       <c r="N48" s="9">
         <v>2</v>
       </c>
-      <c r="O48" s="3"/>
-      <c r="P48" s="1">
+      <c r="O48" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="P48" s="3"/>
+      <c r="Q48" s="1">
         <f t="shared" si="0"/>
         <v>2.0519911504424782</v>
       </c>
     </row>
-    <row r="49" spans="1:19">
+    <row r="49" spans="1:20">
       <c r="A49" s="3" t="s">
         <v>44</v>
       </c>
@@ -3801,25 +3964,28 @@
       <c r="N49" s="9">
         <v>2</v>
       </c>
-      <c r="O49" s="3"/>
-      <c r="P49" s="1">
+      <c r="O49" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="P49" s="3"/>
+      <c r="Q49" s="1">
         <f t="shared" si="0"/>
         <v>1.140123804164322</v>
       </c>
-      <c r="Q49" s="1">
+      <c r="R49" s="1">
         <f t="shared" si="1"/>
         <v>5.9385000000000003</v>
       </c>
-      <c r="R49" s="1">
+      <c r="S49" s="1">
         <f t="shared" si="2"/>
         <v>1526.4856480000003</v>
       </c>
-      <c r="S49" s="1">
+      <c r="T49" s="1">
         <f t="shared" si="3"/>
         <v>3.8903084400306129E-3</v>
       </c>
     </row>
-    <row r="50" spans="1:19">
+    <row r="50" spans="1:20">
       <c r="A50" s="3" t="s">
         <v>45</v>
       </c>
@@ -3860,25 +4026,28 @@
       <c r="N50" s="9">
         <v>2</v>
       </c>
-      <c r="O50" s="3"/>
-      <c r="P50" s="1">
+      <c r="O50" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="P50" s="3"/>
+      <c r="Q50" s="1">
         <f t="shared" si="0"/>
         <v>1.0718588640275388</v>
       </c>
-      <c r="Q50" s="1">
+      <c r="R50" s="1">
         <f t="shared" si="1"/>
         <v>3.1312000000000002</v>
       </c>
-      <c r="R50" s="1">
+      <c r="S50" s="1">
         <f t="shared" si="2"/>
         <v>3010.3236799999995</v>
       </c>
-      <c r="S50" s="1">
+      <c r="T50" s="1">
         <f t="shared" si="3"/>
         <v>1.0401539278992087E-3</v>
       </c>
     </row>
-    <row r="51" spans="1:19">
+    <row r="51" spans="1:20">
       <c r="A51" s="3" t="s">
         <v>46</v>
       </c>
@@ -3908,13 +4077,16 @@
       <c r="N51" s="9">
         <v>1</v>
       </c>
-      <c r="O51" s="3"/>
-      <c r="P51" s="1">
+      <c r="O51" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="P51" s="3"/>
+      <c r="Q51" s="1">
         <f t="shared" si="0"/>
         <v>1.315566323440339</v>
       </c>
     </row>
-    <row r="52" spans="1:19">
+    <row r="52" spans="1:20">
       <c r="A52" s="3" t="s">
         <v>47</v>
       </c>
@@ -3955,25 +4127,28 @@
       <c r="N52" s="9">
         <v>2</v>
       </c>
-      <c r="O52" s="3"/>
-      <c r="P52" s="1">
+      <c r="O52" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="P52" s="3"/>
+      <c r="Q52" s="1">
         <f t="shared" si="0"/>
         <v>1.1965499215891271</v>
       </c>
-      <c r="Q52" s="1">
+      <c r="R52" s="1">
         <f t="shared" si="1"/>
         <v>17.933599999999998</v>
       </c>
-      <c r="R52" s="1">
+      <c r="S52" s="1">
         <f t="shared" si="2"/>
         <v>2128.1245020000001</v>
       </c>
-      <c r="S52" s="1">
+      <c r="T52" s="1">
         <f t="shared" si="3"/>
         <v>8.4269505769733379E-3</v>
       </c>
     </row>
-    <row r="53" spans="1:19">
+    <row r="53" spans="1:20">
       <c r="A53" s="3" t="s">
         <v>48</v>
       </c>
@@ -4014,25 +4189,28 @@
       <c r="N53" s="9">
         <v>2</v>
       </c>
-      <c r="O53" s="3"/>
-      <c r="P53" s="1">
+      <c r="O53" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="P53" s="3"/>
+      <c r="Q53" s="1">
         <f t="shared" si="0"/>
         <v>1.3353293413173652</v>
       </c>
-      <c r="Q53" s="1">
+      <c r="R53" s="1">
         <f t="shared" si="1"/>
         <v>130.96719999999999</v>
       </c>
-      <c r="R53" s="1">
+      <c r="S53" s="1">
         <f t="shared" si="2"/>
         <v>15601.446612</v>
       </c>
-      <c r="S53" s="1">
+      <c r="T53" s="1">
         <f t="shared" si="3"/>
         <v>8.3945548933433735E-3</v>
       </c>
     </row>
-    <row r="54" spans="1:19">
+    <row r="54" spans="1:20">
       <c r="A54" s="3" t="s">
         <v>49</v>
       </c>
@@ -4072,25 +4250,28 @@
       <c r="N54" s="9">
         <v>2</v>
       </c>
-      <c r="O54" s="3"/>
-      <c r="P54" s="1">
+      <c r="O54" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="P54" s="3"/>
+      <c r="Q54" s="1">
         <f t="shared" si="0"/>
         <v>1.3785982478097623</v>
       </c>
-      <c r="Q54" s="1">
+      <c r="R54" s="1">
         <f t="shared" si="1"/>
         <v>10.178100000000001</v>
       </c>
-      <c r="R54" s="1">
+      <c r="S54" s="1">
         <f t="shared" si="2"/>
         <v>2020.7061560000002</v>
       </c>
-      <c r="S54" s="1">
+      <c r="T54" s="1">
         <f t="shared" si="3"/>
         <v>5.0369025549699964E-3</v>
       </c>
     </row>
-    <row r="55" spans="1:19">
+    <row r="55" spans="1:20">
       <c r="A55" s="3" t="s">
         <v>50</v>
       </c>
@@ -4131,25 +4312,28 @@
       <c r="N55" s="9">
         <v>3</v>
       </c>
-      <c r="O55" s="3"/>
-      <c r="P55" s="1">
+      <c r="O55" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="P55" s="3"/>
+      <c r="Q55" s="1">
         <f t="shared" si="0"/>
         <v>1.2076856649395509</v>
       </c>
-      <c r="Q55" s="1">
+      <c r="R55" s="1">
         <f t="shared" si="1"/>
         <v>12.736800000000001</v>
       </c>
-      <c r="R55" s="1">
+      <c r="S55" s="1">
         <f t="shared" si="2"/>
         <v>3582.2521560000005</v>
       </c>
-      <c r="S55" s="1">
+      <c r="T55" s="1">
         <f t="shared" si="3"/>
         <v>3.5555286019346316E-3</v>
       </c>
     </row>
-    <row r="56" spans="1:19">
+    <row r="56" spans="1:20">
       <c r="A56" s="3" t="s">
         <v>51</v>
       </c>
@@ -4179,13 +4363,16 @@
       <c r="N56" s="9">
         <v>2</v>
       </c>
-      <c r="O56" s="3"/>
-      <c r="P56" s="1">
+      <c r="O56" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="P56" s="3"/>
+      <c r="Q56" s="1">
         <f t="shared" si="0"/>
         <v>1.3324764353041989</v>
       </c>
     </row>
-    <row r="57" spans="1:19">
+    <row r="57" spans="1:20">
       <c r="A57" s="3" t="s">
         <v>52</v>
       </c>
@@ -4226,25 +4413,28 @@
       <c r="N57" s="9">
         <v>2</v>
       </c>
-      <c r="O57" s="3"/>
-      <c r="P57" s="1">
+      <c r="O57" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="P57" s="3"/>
+      <c r="Q57" s="1">
         <f t="shared" si="0"/>
         <v>1.1740966682308775</v>
       </c>
-      <c r="Q57" s="1">
+      <c r="R57" s="1">
         <f t="shared" si="1"/>
         <v>16.620799999999999</v>
       </c>
-      <c r="R57" s="1">
+      <c r="S57" s="1">
         <f t="shared" si="2"/>
         <v>3295.0289159999998</v>
       </c>
-      <c r="S57" s="1">
+      <c r="T57" s="1">
         <f t="shared" si="3"/>
         <v>5.0442045953808558E-3</v>
       </c>
     </row>
-    <row r="58" spans="1:19">
+    <row r="58" spans="1:20">
       <c r="A58" s="3" t="s">
         <v>53</v>
       </c>
@@ -4274,13 +4464,16 @@
       <c r="N58" s="9">
         <v>3</v>
       </c>
-      <c r="O58" s="3"/>
-      <c r="P58" s="1">
+      <c r="O58" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="P58" s="3"/>
+      <c r="Q58" s="1">
         <f t="shared" si="0"/>
         <v>1.0652346857597454</v>
       </c>
     </row>
-    <row r="59" spans="1:19">
+    <row r="59" spans="1:20">
       <c r="A59" s="3" t="s">
         <v>54</v>
       </c>
@@ -4321,25 +4514,28 @@
       <c r="N59" s="9">
         <v>2</v>
       </c>
-      <c r="O59" s="3"/>
-      <c r="P59" s="1">
+      <c r="O59" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="P59" s="3"/>
+      <c r="Q59" s="1">
         <f t="shared" si="0"/>
         <v>1.1102082275266631</v>
       </c>
-      <c r="Q59" s="1">
+      <c r="R59" s="1">
         <f t="shared" si="1"/>
         <v>19.066199999999998</v>
       </c>
-      <c r="R59" s="1">
+      <c r="S59" s="1">
         <f t="shared" si="2"/>
         <v>1988.5561080000002</v>
       </c>
-      <c r="S59" s="1">
+      <c r="T59" s="1">
         <f t="shared" si="3"/>
         <v>9.5879617996677598E-3</v>
       </c>
     </row>
-    <row r="60" spans="1:19">
+    <row r="60" spans="1:20">
       <c r="A60" s="3" t="s">
         <v>55</v>
       </c>
@@ -4380,25 +4576,28 @@
       <c r="N60" s="9">
         <v>2</v>
       </c>
-      <c r="O60" s="3"/>
-      <c r="P60" s="1">
+      <c r="O60" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="P60" s="3"/>
+      <c r="Q60" s="1">
         <f t="shared" si="0"/>
         <v>1.2215239591516105</v>
       </c>
-      <c r="Q60" s="1">
+      <c r="R60" s="1">
         <f t="shared" si="1"/>
         <v>27.442800000000002</v>
       </c>
-      <c r="R60" s="1">
+      <c r="S60" s="1">
         <f t="shared" si="2"/>
         <v>5986.0533599999999</v>
       </c>
-      <c r="S60" s="1">
+      <c r="T60" s="1">
         <f t="shared" si="3"/>
         <v>4.5844562935870659E-3</v>
       </c>
     </row>
-    <row r="61" spans="1:19">
+    <row r="61" spans="1:20">
       <c r="A61" s="4" t="s">
         <v>56</v>
       </c>
@@ -4439,26 +4638,39 @@
       <c r="N61" s="12">
         <v>2</v>
       </c>
-      <c r="O61" s="4"/>
-      <c r="P61" s="1">
+      <c r="O61" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="P61" s="4"/>
+      <c r="Q61" s="1">
         <f t="shared" si="0"/>
         <v>1.2775229357798166</v>
       </c>
-      <c r="Q61" s="1">
+      <c r="R61" s="1">
         <f>H61*I61</f>
         <v>121.8021</v>
       </c>
-      <c r="R61" s="1">
+      <c r="S61" s="1">
         <f t="shared" si="2"/>
         <v>6040.9434999999994</v>
       </c>
-      <c r="S61" s="1">
+      <c r="T61" s="1">
         <f t="shared" si="3"/>
         <v>2.0162760999171737E-2</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="18">
+  <mergeCells count="19">
+    <mergeCell ref="P1:P4"/>
+    <mergeCell ref="H2:H4"/>
+    <mergeCell ref="I2:I4"/>
+    <mergeCell ref="J2:J4"/>
+    <mergeCell ref="K2:K4"/>
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="N2:N4"/>
+    <mergeCell ref="L3:L4"/>
+    <mergeCell ref="M3:M4"/>
+    <mergeCell ref="O1:O4"/>
     <mergeCell ref="A1:A4"/>
     <mergeCell ref="F1:F4"/>
     <mergeCell ref="G1:K1"/>
@@ -4468,15 +4680,6 @@
     <mergeCell ref="D1:D4"/>
     <mergeCell ref="C1:C4"/>
     <mergeCell ref="B1:B4"/>
-    <mergeCell ref="O1:O4"/>
-    <mergeCell ref="H2:H4"/>
-    <mergeCell ref="I2:I4"/>
-    <mergeCell ref="J2:J4"/>
-    <mergeCell ref="K2:K4"/>
-    <mergeCell ref="L2:M2"/>
-    <mergeCell ref="N2:N4"/>
-    <mergeCell ref="L3:L4"/>
-    <mergeCell ref="M3:M4"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <dataValidations count="1">

</xml_diff>